<commit_message>
Modified POM classes and Test case for Exercise 2
</commit_message>
<xml_diff>
--- a/src/test/resources/Driver/DataDriver.xlsx
+++ b/src/test/resources/Driver/DataDriver.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\AgileInternship\Selenium\Clone\Ejercicio2\Selenium-Exercise1\src\test\resources\Driver\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7A0513-0DA5-4A41-B9D9-E6EFF1BB427D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="16515" windowHeight="5205"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,55 +22,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>No</t>
+    <t>intern6@agilethought.com</t>
   </si>
   <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>CurrentAddress</t>
-  </si>
-  <si>
-    <t>PermanentAddress</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>tester1@test.com</t>
-  </si>
-  <si>
-    <t>Permanent Test Address 1</t>
-  </si>
-  <si>
-    <t>Current Test Address 1</t>
-  </si>
-  <si>
-    <t>Current Test Address 2</t>
-  </si>
-  <si>
-    <t>Permanent Test Address 2</t>
+    <t>P@ssw0rd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,7 +65,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,22 +76,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E3" totalsRowShown="0">
-  <autoFilter ref="A1:E3"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="No"/>
-    <tableColumn id="2" name="FullName"/>
-    <tableColumn id="3" name="Email"/>
-    <tableColumn id="4" name="CurrentAddress"/>
-    <tableColumn id="5" name="PermanentAddress"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -166,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,9 +159,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,6 +211,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,88 +403,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="5" width="34" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -502,7 +440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>